<commit_message>
Ready for train test split paraphrased
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/classification_wo_paraphrase_report.xlsx
+++ b/textToOps/data/processed/classification_wo_paraphrase_report.xlsx
@@ -465,13 +465,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8484848484848485</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.9859154929577464</v>
       </c>
       <c r="E6" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -560,13 +560,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -579,13 +579,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.8148148148148148</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.878048780487805</v>
+        <v>0.8979591836734693</v>
       </c>
       <c r="E9" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -617,13 +617,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.8</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8823529411764706</v>
+        <v>0.9</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9375</v>
+        <v>0.9473684210526316</v>
       </c>
       <c r="E12" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -693,13 +693,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -718,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -731,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9565217391304348</v>
+        <v>0.962962962962963</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -747,16 +747,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -769,13 +769,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.875</v>
       </c>
       <c r="D18" t="n">
-        <v>0.923076923076923</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -807,13 +807,13 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -880,16 +880,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -899,16 +899,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9465020576131687</v>
+        <v>0.9297658862876255</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9465020576131687</v>
+        <v>0.9297658862876255</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9465020576131687</v>
+        <v>0.9297658862876255</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9465020576131687</v>
+        <v>0.9297658862876255</v>
       </c>
     </row>
     <row r="26">
@@ -918,16 +918,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9414717619877188</v>
+        <v>0.9336018970609764</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9251897860593512</v>
+        <v>0.8805077169207604</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9289572082623522</v>
+        <v>0.8870649772157809</v>
       </c>
       <c r="E26" t="n">
-        <v>243</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27">
@@ -937,16 +937,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9536352335411411</v>
+        <v>0.9448668930766118</v>
       </c>
       <c r="C27" t="n">
-        <v>0.9465020576131687</v>
+        <v>0.9297658862876255</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9458877451460398</v>
+        <v>0.9280713624955823</v>
       </c>
       <c r="E27" t="n">
-        <v>243</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>